<commit_message>
add keyboard aware scroll feature to features doc
</commit_message>
<xml_diff>
--- a/doc/features.xlsx
+++ b/doc/features.xlsx
@@ -27,6 +27,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">一级</t>
     </r>
@@ -35,6 +36,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">screen</t>
     </r>
@@ -45,6 +47,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">二级</t>
     </r>
@@ -53,6 +56,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">screen</t>
     </r>
@@ -90,6 +94,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">标志</t>
     </r>
@@ -98,6 +103,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Icon</t>
     </r>
@@ -106,6 +112,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">与提示进入任务详情</t>
     </r>
@@ -114,6 +121,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Icon</t>
     </r>
@@ -124,6 +132,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">支持进入任务详情</t>
     </r>
@@ -132,6 +141,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">navigate</t>
     </r>
@@ -157,6 +167,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">scan</t>
     </r>
@@ -165,6 +176,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">动画</t>
     </r>
@@ -175,6 +187,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">显示正在读取</t>
     </r>
@@ -183,6 +196,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RFID</t>
     </r>
@@ -191,6 +205,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">动画</t>
     </r>
@@ -204,6 +219,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">调用手机</t>
     </r>
@@ -212,6 +228,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NFC</t>
     </r>
@@ -220,6 +237,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">功能，读取</t>
     </r>
@@ -228,6 +246,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RFID</t>
     </r>
@@ -236,6 +255,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">信息</t>
     </r>
@@ -246,6 +266,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">当读取到</t>
     </r>
@@ -254,6 +275,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RFID</t>
     </r>
@@ -262,6 +284,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">信息时，发出“滴”的提示音，并进入查找信息动画</t>
     </r>
@@ -275,6 +298,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">从后端服务器获取该标签的信息，包含：设施信息，关联的任务信息，关联的任务检测模板；
 如果该</t>
@@ -284,6 +308,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RFID</t>
     </r>
@@ -292,6 +317,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">查找到相关设施，并且该设施包含在某些未完成任务中，获取其中最早创建的任务信息，并进入检测详情</t>
     </r>
@@ -300,6 +326,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">screen</t>
     </r>
@@ -310,6 +337,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">显示提示信息：未找到</t>
     </r>
@@ -318,6 +346,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RFID</t>
     </r>
@@ -326,6 +355,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">信息</t>
     </r>
@@ -336,6 +366,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">如果未在后端服务器查找到该</t>
     </r>
@@ -344,6 +375,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RFID</t>
     </r>
@@ -352,6 +384,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">设施信息，显示提示信息，用户点屏后再进入读取</t>
     </r>
@@ -360,6 +393,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RFID</t>
     </r>
@@ -368,6 +402,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">动画</t>
     </r>
@@ -381,6 +416,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">如果该</t>
     </r>
@@ -389,6 +425,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">RFID</t>
     </r>
@@ -397,6 +434,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">未关联任何未完成任务，显示提示信息，用户可点击选择返回或查看设施详情</t>
     </r>
@@ -419,6 +457,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">点击添加备注图标，显示该步骤</t>
     </r>
@@ -427,6 +466,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">card</t>
     </r>
@@ -435,8 +475,9 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">出现文本输入框，文本输入框支持自动缩放</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">出现文本输入框，文本输入框支持自动缩放，并支持键盘感知自动滚屏</t>
     </r>
   </si>
   <si>
@@ -454,6 +495,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">在该执行步骤</t>
     </r>
@@ -462,6 +504,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">card</t>
     </r>
@@ -470,6 +513,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">中显示照片，位置在备注后</t>
     </r>
@@ -483,6 +527,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">任务执行步骤最后有提交报告</t>
     </r>
@@ -491,6 +536,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">button</t>
     </r>
@@ -499,6 +545,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">，点击后首先检查任务执行是否完成，如未完成（如某些执行步骤未输入检测结果）显示提示信息；如果任务执行完成，则向后端服务器上传任务执行报告信息，</t>
     </r>
@@ -507,6 +554,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">screen</t>
     </r>
@@ -515,6 +563,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">显示数据上传动画</t>
     </r>
@@ -528,6 +577,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">等待服务器返回信息，如果成功则显示提示信息：报告提交成功，用户点击确定后返回</t>
     </r>
@@ -536,6 +586,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">scan</t>
     </r>
@@ -544,6 +595,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">动画</t>
     </r>
@@ -552,6 +604,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">screen</t>
     </r>
@@ -560,6 +613,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">；如果超时则显示提示信息，上传失败，用户确定后返回检测详情</t>
     </r>
@@ -568,6 +622,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">screen</t>
     </r>
@@ -599,6 +654,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">显示用户名、</t>
     </r>
@@ -607,6 +663,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">email</t>
     </r>
@@ -615,6 +672,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">、完成任务总数、未完成任务总数、逾期任务总数</t>
     </r>
@@ -631,6 +689,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">用户</t>
     </r>
@@ -639,6 +698,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">email</t>
     </r>
@@ -647,6 +707,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">（用户名），密码。登录成功进入首页</t>
     </r>
@@ -655,6 +716,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">screen</t>
     </r>
@@ -663,6 +725,7 @@
         <sz val="10"/>
         <rFont val="Noto Sans CJK SC Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">；登录失败提示失败信息。</t>
     </r>
@@ -680,6 +743,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -700,6 +764,7 @@
       <sz val="10"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -785,15 +850,15 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="96.5663265306123"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="95.4387755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fix features doc, add upload feature in FacilituList component, add some data in datasource
</commit_message>
<xml_diff>
--- a/doc/features.xlsx
+++ b/doc/features.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="54">
   <si>
     <r>
       <rPr>
@@ -156,7 +156,7 @@
     <t xml:space="preserve">显示任务内容、开始时间、结束时间与备注信息</t>
   </si>
   <si>
-    <t xml:space="preserve">显示任务包含的设施列表</t>
+    <t xml:space="preserve">显示任务包含的设施列表，首部icon显示每项设施状态：已完成任务并已提交服务器成功、已完成任务但未提交服务器成功、未完成任务；当状态为已完成任务但未提交服务器成功时，尾部出现提交icon，点击后出现提交动画，成功后显示已提交成功icon，首部icon状态变为已完成任务并已提交服务器成功的icon，提交失败则重新变为提交icon</t>
   </si>
   <si>
     <t xml:space="preserve">检测</t>
@@ -300,8 +300,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">从后端服务器获取该标签的信息，包含：设施信息，关联的任务信息，关联的任务检测模板；
-如果该</t>
+      <t xml:space="preserve">从redux state中取该标签的信息，如果该</t>
     </r>
     <r>
       <rPr>
@@ -368,7 +367,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">如果未在后端服务器查找到该</t>
+      <t xml:space="preserve">如果未查找到该</t>
     </r>
     <r>
       <rPr>
@@ -386,7 +385,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">设施信息，显示提示信息，用户点屏后再进入读取</t>
+      <t xml:space="preserve">设施信息，显示提示信息，用户点屏后重新回到读取</t>
     </r>
     <r>
       <rPr>
@@ -446,6 +445,35 @@
     <t xml:space="preserve">显示任务详情：任务执行详细步骤</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">如果该</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">RFID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">关联的任务已完成但未提交，则显示已完成任务的详情，可直接提交或修改后提交</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">根据该任务关联的任务模板，显示任务执行的每一个步骤，每一步骤分别显示执行要求、合格与不合格选项、添加备注与拍照功能</t>
   </si>
   <si>
@@ -615,7 +643,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">；如果超时则显示提示信息，上传失败，用户确定后返回检测详情</t>
+      <t xml:space="preserve">；如果超时则显示提示信息，上传失败，任务执行信息已保存，请在该任务详情中再次提交，用户确定后返回检测动画</t>
     </r>
     <r>
       <rPr>
@@ -847,18 +875,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="95.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="93.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -963,7 +991,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="66.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1031,7 +1059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="48.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="34.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1065,7 +1093,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1082,7 +1110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="32.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1099,7 +1127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1107,44 +1135,44 @@
         <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="E17" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="32.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1152,10 +1180,10 @@
         <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>9</v>
@@ -1169,27 +1197,27 @@
         <v>29</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="49.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>9</v>
@@ -1197,16 +1225,16 @@
     </row>
     <row r="21" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>9</v>
@@ -1214,18 +1242,35 @@
     </row>
     <row r="22" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="E22" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="D23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modify the feature doc, modify the check record implementation plan
</commit_message>
<xml_diff>
--- a/doc/features.xlsx
+++ b/doc/features.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
   <si>
     <r>
       <rPr>
@@ -477,36 +477,13 @@
     <t xml:space="preserve">根据该任务关联的任务模板，显示任务执行的每一个步骤，每一步骤分别显示执行要求、合格与不合格选项、添加备注与拍照功能</t>
   </si>
   <si>
-    <t xml:space="preserve">添加备注</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">点击添加备注图标，显示该步骤</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">card</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Noto Sans CJK SC Regular"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">出现文本输入框，文本输入框支持自动缩放，并支持键盘感知自动滚屏</t>
-    </r>
+    <t xml:space="preserve">检测记录</t>
+  </si>
+  <si>
+    <t xml:space="preserve">添加检测记录</t>
+  </si>
+  <si>
+    <t xml:space="preserve">点击添加备注图标，进入检测记录screen，支持用户录入文档，点击确定后提交文档，并返回检测详情screen</t>
   </si>
   <si>
     <t xml:space="preserve">拍照</t>
@@ -878,15 +855,15 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="93.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="92.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,18 +1121,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>9</v>
@@ -1163,10 +1140,10 @@
     </row>
     <row r="17" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>9</v>
@@ -1180,10 +1157,10 @@
         <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E18" s="0" t="s">
         <v>9</v>
@@ -1197,10 +1174,10 @@
         <v>29</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>9</v>
@@ -1214,10 +1191,10 @@
         <v>29</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="0" t="s">
         <v>9</v>
@@ -1225,16 +1202,16 @@
     </row>
     <row r="21" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>9</v>
@@ -1242,16 +1219,16 @@
     </row>
     <row r="22" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>9</v>
@@ -1259,16 +1236,16 @@
     </row>
     <row r="23" customFormat="false" ht="16.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>9</v>

</xml_diff>